<commit_message>
- Done till MaxSquare - MaxLengthChain is remaining
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="843">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -2416,16 +2416,31 @@
     <t xml:space="preserve">Longest subsequence such that difference between adjacent is one</t>
   </si>
   <si>
+    <t xml:space="preserve">Perform LIS with condition being difference = 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum subsequence sum such that no three are consecutive</t>
   </si>
   <si>
+    <t xml:space="preserve">similar to no 2 adjacent except handle 3 cases starting from I = 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Egg Dropping Problem</t>
   </si>
   <si>
+    <t xml:space="preserve">Choose best of worst =&gt; f(e, f) = min(max(f(e, f-k), f(e-1,k-1)) for k=0 to f-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum Length Chain of Pairs</t>
   </si>
   <si>
+    <t xml:space="preserve">perform LIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum size square sub-matrix with all 1s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bottom up 1d DP like Lcs</t>
   </si>
   <si>
     <t xml:space="preserve">Maximum sum of pairs with specific difference</t>
@@ -3098,8 +3113,8 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D426" activeCellId="0" sqref="D426"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A412" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D435" activeCellId="0" sqref="D435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7613,14 +7628,14 @@
         <v>784</v>
       </c>
     </row>
-    <row r="429" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B429" s="5" t="s">
         <v>747</v>
       </c>
       <c r="C429" s="6" t="s">
         <v>785</v>
       </c>
-      <c r="D429" s="11" t="s">
+      <c r="D429" s="7" t="s">
         <v>786</v>
       </c>
     </row>
@@ -7631,8 +7646,8 @@
       <c r="C430" s="6" t="s">
         <v>787</v>
       </c>
-      <c r="D430" s="10" t="s">
-        <v>71</v>
+      <c r="D430" s="7" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7640,10 +7655,10 @@
         <v>747</v>
       </c>
       <c r="C431" s="6" t="s">
-        <v>788</v>
-      </c>
-      <c r="D431" s="10" t="s">
-        <v>71</v>
+        <v>789</v>
+      </c>
+      <c r="D431" s="7" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7651,21 +7666,21 @@
         <v>747</v>
       </c>
       <c r="C432" s="6" t="s">
-        <v>789</v>
-      </c>
-      <c r="D432" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="433" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>791</v>
+      </c>
+      <c r="D432" s="7" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B433" s="5" t="s">
         <v>747</v>
       </c>
       <c r="C433" s="6" t="s">
-        <v>790</v>
-      </c>
-      <c r="D433" s="10" t="s">
-        <v>71</v>
+        <v>793</v>
+      </c>
+      <c r="D433" s="11" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7673,10 +7688,10 @@
         <v>747</v>
       </c>
       <c r="C434" s="6" t="s">
-        <v>791</v>
-      </c>
-      <c r="D434" s="10" t="s">
-        <v>71</v>
+        <v>795</v>
+      </c>
+      <c r="D434" s="7" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7684,9 +7699,9 @@
         <v>747</v>
       </c>
       <c r="C435" s="6" t="s">
-        <v>792</v>
-      </c>
-      <c r="D435" s="10" t="s">
+        <v>797</v>
+      </c>
+      <c r="D435" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7695,9 +7710,9 @@
         <v>747</v>
       </c>
       <c r="C436" s="6" t="s">
-        <v>793</v>
-      </c>
-      <c r="D436" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="D436" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7706,9 +7721,9 @@
         <v>747</v>
       </c>
       <c r="C437" s="6" t="s">
-        <v>794</v>
-      </c>
-      <c r="D437" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="D437" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7717,9 +7732,9 @@
         <v>747</v>
       </c>
       <c r="C438" s="6" t="s">
-        <v>795</v>
-      </c>
-      <c r="D438" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="D438" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7728,9 +7743,9 @@
         <v>747</v>
       </c>
       <c r="C439" s="6" t="s">
-        <v>796</v>
-      </c>
-      <c r="D439" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="D439" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7739,7 +7754,7 @@
         <v>747</v>
       </c>
       <c r="C440" s="6" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="D440" s="10" t="s">
         <v>71</v>
@@ -7750,7 +7765,7 @@
         <v>747</v>
       </c>
       <c r="C441" s="6" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="D441" s="10" t="s">
         <v>71</v>
@@ -7761,7 +7776,7 @@
         <v>747</v>
       </c>
       <c r="C442" s="6" t="s">
-        <v>799</v>
+        <v>804</v>
       </c>
       <c r="D442" s="10" t="s">
         <v>71</v>
@@ -7772,7 +7787,7 @@
         <v>747</v>
       </c>
       <c r="C443" s="6" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="D443" s="10" t="s">
         <v>71</v>
@@ -7783,7 +7798,7 @@
         <v>747</v>
       </c>
       <c r="C444" s="6" t="s">
-        <v>801</v>
+        <v>806</v>
       </c>
       <c r="D444" s="10" t="s">
         <v>71</v>
@@ -7794,7 +7809,7 @@
         <v>747</v>
       </c>
       <c r="C445" s="6" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="D445" s="10" t="s">
         <v>71</v>
@@ -7805,7 +7820,7 @@
         <v>747</v>
       </c>
       <c r="C446" s="6" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
       <c r="D446" s="10" t="s">
         <v>71</v>
@@ -7816,7 +7831,7 @@
         <v>747</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="D447" s="10" t="s">
         <v>71</v>
@@ -7827,7 +7842,7 @@
         <v>747</v>
       </c>
       <c r="C448" s="6" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="D448" s="10" t="s">
         <v>71</v>
@@ -7838,7 +7853,7 @@
         <v>747</v>
       </c>
       <c r="C449" s="6" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="D449" s="10" t="s">
         <v>71</v>
@@ -7849,7 +7864,7 @@
         <v>747</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="D450" s="10" t="s">
         <v>71</v>
@@ -7860,7 +7875,7 @@
         <v>747</v>
       </c>
       <c r="C451" s="6" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="D451" s="10" t="s">
         <v>71</v>
@@ -7871,7 +7886,7 @@
         <v>747</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>809</v>
+        <v>814</v>
       </c>
       <c r="D452" s="10" t="s">
         <v>71</v>
@@ -7882,7 +7897,7 @@
         <v>747</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>810</v>
+        <v>815</v>
       </c>
       <c r="D453" s="10" t="s">
         <v>71</v>
@@ -7893,7 +7908,7 @@
         <v>747</v>
       </c>
       <c r="C454" s="6" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="D454" s="10" t="s">
         <v>71</v>
@@ -7904,7 +7919,7 @@
         <v>747</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>812</v>
+        <v>817</v>
       </c>
       <c r="D455" s="10" t="s">
         <v>71</v>
@@ -7915,7 +7930,7 @@
         <v>747</v>
       </c>
       <c r="C456" s="6" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="D456" s="10" t="s">
         <v>71</v>
@@ -7926,7 +7941,7 @@
         <v>747</v>
       </c>
       <c r="C457" s="6" t="s">
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="D457" s="10" t="s">
         <v>71</v>
@@ -7937,7 +7952,7 @@
         <v>747</v>
       </c>
       <c r="C458" s="6" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="D458" s="10" t="s">
         <v>71</v>
@@ -7948,7 +7963,7 @@
         <v>747</v>
       </c>
       <c r="C459" s="6" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="D459" s="10" t="s">
         <v>71</v>
@@ -7959,7 +7974,7 @@
         <v>747</v>
       </c>
       <c r="C460" s="6" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="D460" s="10" t="s">
         <v>71</v>
@@ -7970,7 +7985,7 @@
         <v>747</v>
       </c>
       <c r="C461" s="6" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="D461" s="10" t="s">
         <v>71</v>
@@ -7981,7 +7996,7 @@
         <v>747</v>
       </c>
       <c r="C462" s="6" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="D462" s="10" t="s">
         <v>71</v>
@@ -7992,7 +8007,7 @@
         <v>747</v>
       </c>
       <c r="C463" s="6" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="D463" s="10" t="s">
         <v>71</v>
@@ -8003,7 +8018,7 @@
         <v>747</v>
       </c>
       <c r="C464" s="6" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="D464" s="10" t="s">
         <v>71</v>
@@ -8014,7 +8029,7 @@
         <v>747</v>
       </c>
       <c r="C465" s="6" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="D465" s="10" t="s">
         <v>71</v>
@@ -8025,7 +8040,7 @@
         <v>747</v>
       </c>
       <c r="C466" s="6" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="D466" s="10" t="s">
         <v>71</v>
@@ -8036,7 +8051,7 @@
         <v>747</v>
       </c>
       <c r="C467" s="6" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
       <c r="D467" s="10" t="s">
         <v>71</v>
@@ -8047,7 +8062,7 @@
         <v>747</v>
       </c>
       <c r="C468" s="6" t="s">
-        <v>825</v>
+        <v>830</v>
       </c>
       <c r="D468" s="10" t="s">
         <v>71</v>
@@ -8058,7 +8073,7 @@
         <v>747</v>
       </c>
       <c r="C469" s="6" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="D469" s="10" t="s">
         <v>71</v>
@@ -8075,10 +8090,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B472" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="D472" s="10" t="s">
         <v>71</v>
@@ -8086,10 +8101,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B473" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C473" s="6" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="D473" s="10" t="s">
         <v>71</v>
@@ -8097,10 +8112,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B474" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C474" s="6" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="D474" s="10" t="s">
         <v>71</v>
@@ -8108,10 +8123,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B475" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C475" s="6" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="D475" s="10" t="s">
         <v>71</v>
@@ -8119,10 +8134,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B476" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C476" s="6" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="D476" s="10" t="s">
         <v>71</v>
@@ -8130,10 +8145,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B477" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C477" s="6" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="D477" s="10" t="s">
         <v>71</v>
@@ -8141,10 +8156,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B478" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C478" s="6" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="D478" s="10" t="s">
         <v>71</v>
@@ -8152,10 +8167,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B479" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C479" s="6" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="D479" s="10" t="s">
         <v>71</v>
@@ -8163,10 +8178,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B480" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C480" s="6" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="D480" s="10" t="s">
         <v>71</v>
@@ -8174,10 +8189,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="5" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="C481" s="6" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="D481" s="10" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Finished Till ContiguousSubArrayWithMaxSum using Kadane's Algorithm
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="853">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -2476,16 +2476,31 @@
     <t xml:space="preserve">Minimum removals from array to make max –min &lt;= K</t>
   </si>
   <si>
+    <t xml:space="preserve">sort then for each element find the next greater element with diff &lt;= k</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longest Common Substring</t>
   </si>
   <si>
+    <t xml:space="preserve">Curr = prev + 1 or 0, result is maximum of curr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count number of ways to reacha given score in a game</t>
   </si>
   <si>
+    <t xml:space="preserve">it’s coin change permutation problem</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Balanced Binary Trees of Height h</t>
   </si>
   <si>
+    <t xml:space="preserve">balanced tree h has 3 subtree cases, (h-1, h-2), (h-2, h-1), (h-2, h-2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">LargestSum Contiguous Subarray [V&gt;V&gt;V&gt;V IMP ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use kadane’s algorithm</t>
   </si>
   <si>
     <t xml:space="preserve">Smallest sum contiguous subarray</t>
@@ -3128,8 +3143,8 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A424" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D437" activeCellId="0" sqref="D437"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A427" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D445" activeCellId="0" sqref="D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7771,8 +7786,8 @@
       <c r="C440" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="D440" s="11" t="s">
-        <v>71</v>
+      <c r="D440" s="7" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7780,10 +7795,10 @@
         <v>747</v>
       </c>
       <c r="C441" s="6" t="s">
-        <v>808</v>
-      </c>
-      <c r="D441" s="11" t="s">
-        <v>71</v>
+        <v>809</v>
+      </c>
+      <c r="D441" s="7" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7791,10 +7806,10 @@
         <v>747</v>
       </c>
       <c r="C442" s="6" t="s">
-        <v>809</v>
-      </c>
-      <c r="D442" s="11" t="s">
-        <v>71</v>
+        <v>811</v>
+      </c>
+      <c r="D442" s="7" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7802,10 +7817,10 @@
         <v>747</v>
       </c>
       <c r="C443" s="6" t="s">
-        <v>810</v>
-      </c>
-      <c r="D443" s="11" t="s">
-        <v>71</v>
+        <v>813</v>
+      </c>
+      <c r="D443" s="7" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7813,10 +7828,10 @@
         <v>747</v>
       </c>
       <c r="C444" s="6" t="s">
-        <v>811</v>
-      </c>
-      <c r="D444" s="11" t="s">
-        <v>71</v>
+        <v>815</v>
+      </c>
+      <c r="D444" s="7" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7824,9 +7839,9 @@
         <v>747</v>
       </c>
       <c r="C445" s="6" t="s">
-        <v>812</v>
-      </c>
-      <c r="D445" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="D445" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7835,9 +7850,9 @@
         <v>747</v>
       </c>
       <c r="C446" s="6" t="s">
-        <v>813</v>
-      </c>
-      <c r="D446" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="D446" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7846,9 +7861,9 @@
         <v>747</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>814</v>
-      </c>
-      <c r="D447" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="D447" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7857,9 +7872,9 @@
         <v>747</v>
       </c>
       <c r="C448" s="6" t="s">
-        <v>815</v>
-      </c>
-      <c r="D448" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="D448" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7868,9 +7883,9 @@
         <v>747</v>
       </c>
       <c r="C449" s="6" t="s">
-        <v>816</v>
-      </c>
-      <c r="D449" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="D449" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7879,7 +7894,7 @@
         <v>747</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="D450" s="10" t="s">
         <v>71</v>
@@ -7890,7 +7905,7 @@
         <v>747</v>
       </c>
       <c r="C451" s="6" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="D451" s="10" t="s">
         <v>71</v>
@@ -7901,7 +7916,7 @@
         <v>747</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="D452" s="10" t="s">
         <v>71</v>
@@ -7912,7 +7927,7 @@
         <v>747</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="D453" s="10" t="s">
         <v>71</v>
@@ -7923,7 +7938,7 @@
         <v>747</v>
       </c>
       <c r="C454" s="6" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="D454" s="10" t="s">
         <v>71</v>
@@ -7934,7 +7949,7 @@
         <v>747</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="D455" s="10" t="s">
         <v>71</v>
@@ -7945,7 +7960,7 @@
         <v>747</v>
       </c>
       <c r="C456" s="6" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="D456" s="10" t="s">
         <v>71</v>
@@ -7956,7 +7971,7 @@
         <v>747</v>
       </c>
       <c r="C457" s="6" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
       <c r="D457" s="10" t="s">
         <v>71</v>
@@ -7967,7 +7982,7 @@
         <v>747</v>
       </c>
       <c r="C458" s="6" t="s">
-        <v>825</v>
+        <v>830</v>
       </c>
       <c r="D458" s="10" t="s">
         <v>71</v>
@@ -7978,7 +7993,7 @@
         <v>747</v>
       </c>
       <c r="C459" s="6" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="D459" s="10" t="s">
         <v>71</v>
@@ -7989,7 +8004,7 @@
         <v>747</v>
       </c>
       <c r="C460" s="6" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="D460" s="10" t="s">
         <v>71</v>
@@ -8000,7 +8015,7 @@
         <v>747</v>
       </c>
       <c r="C461" s="6" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="D461" s="10" t="s">
         <v>71</v>
@@ -8011,7 +8026,7 @@
         <v>747</v>
       </c>
       <c r="C462" s="6" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="D462" s="10" t="s">
         <v>71</v>
@@ -8022,7 +8037,7 @@
         <v>747</v>
       </c>
       <c r="C463" s="6" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="D463" s="10" t="s">
         <v>71</v>
@@ -8033,7 +8048,7 @@
         <v>747</v>
       </c>
       <c r="C464" s="6" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="D464" s="10" t="s">
         <v>71</v>
@@ -8044,7 +8059,7 @@
         <v>747</v>
       </c>
       <c r="C465" s="6" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="D465" s="10" t="s">
         <v>71</v>
@@ -8055,7 +8070,7 @@
         <v>747</v>
       </c>
       <c r="C466" s="6" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="D466" s="10" t="s">
         <v>71</v>
@@ -8066,7 +8081,7 @@
         <v>747</v>
       </c>
       <c r="C467" s="6" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="D467" s="10" t="s">
         <v>71</v>
@@ -8077,7 +8092,7 @@
         <v>747</v>
       </c>
       <c r="C468" s="6" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="D468" s="10" t="s">
         <v>71</v>
@@ -8088,7 +8103,7 @@
         <v>747</v>
       </c>
       <c r="C469" s="6" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="D469" s="10" t="s">
         <v>71</v>
@@ -8105,10 +8120,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B472" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="D472" s="10" t="s">
         <v>71</v>
@@ -8116,10 +8131,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B473" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C473" s="6" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="D473" s="10" t="s">
         <v>71</v>
@@ -8127,10 +8142,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B474" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C474" s="6" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="D474" s="10" t="s">
         <v>71</v>
@@ -8138,10 +8153,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B475" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C475" s="6" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="D475" s="10" t="s">
         <v>71</v>
@@ -8149,10 +8164,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B476" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C476" s="6" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="D476" s="10" t="s">
         <v>71</v>
@@ -8160,10 +8175,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B477" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C477" s="6" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="D477" s="10" t="s">
         <v>71</v>
@@ -8171,10 +8186,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B478" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C478" s="6" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="D478" s="10" t="s">
         <v>71</v>
@@ -8182,10 +8197,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B479" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C479" s="6" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="D479" s="10" t="s">
         <v>71</v>
@@ -8193,10 +8208,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B480" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C480" s="6" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="D480" s="10" t="s">
         <v>71</v>
@@ -8204,10 +8219,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="5" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C481" s="6" t="s">
-        <v>847</v>
+        <v>852</v>
       </c>
       <c r="D481" s="10" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
- Done till CheckIfStringIsInterleaved. - ChainPair remaining from DP section.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="876">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -2623,13 +2623,25 @@
     <t xml:space="preserve">Largest area rectangular sub-matrix with equal number of 1’s and 0’s [ IMP ]</t>
   </si>
   <si>
+    <t xml:space="preserve">Take 1 as 1 and 0 as -1, then perform largest area rectangle with sum zero</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum sum rectangle in a 2D matrix</t>
   </si>
   <si>
+    <t xml:space="preserve">similar to largestsumrectangle but use kadane’s algorithm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum profit by buying and selling a share at most k times</t>
   </si>
   <si>
+    <t xml:space="preserve">subproblem is the maxprofit upto k transaction using n days</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find if a string is interleaved of two other strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use topdown approach using NxM matrix for memoization</t>
   </si>
   <si>
     <t xml:space="preserve">Maximum Length of Pair Chain</t>
@@ -3201,7 +3213,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A451" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D462" activeCellId="0" sqref="D462"/>
+      <selection pane="topLeft" activeCell="D470" activeCellId="0" sqref="D470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8118,8 +8130,8 @@
       <c r="C465" s="6" t="s">
         <v>856</v>
       </c>
-      <c r="D465" s="11" t="s">
-        <v>71</v>
+      <c r="D465" s="7" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8127,10 +8139,10 @@
         <v>747</v>
       </c>
       <c r="C466" s="6" t="s">
-        <v>857</v>
-      </c>
-      <c r="D466" s="11" t="s">
-        <v>71</v>
+        <v>858</v>
+      </c>
+      <c r="D466" s="7" t="s">
+        <v>859</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8138,10 +8150,10 @@
         <v>747</v>
       </c>
       <c r="C467" s="6" t="s">
-        <v>858</v>
-      </c>
-      <c r="D467" s="11" t="s">
-        <v>71</v>
+        <v>860</v>
+      </c>
+      <c r="D467" s="7" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8149,10 +8161,10 @@
         <v>747</v>
       </c>
       <c r="C468" s="6" t="s">
-        <v>859</v>
-      </c>
-      <c r="D468" s="11" t="s">
-        <v>71</v>
+        <v>862</v>
+      </c>
+      <c r="D468" s="7" t="s">
+        <v>863</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8160,7 +8172,7 @@
         <v>747</v>
       </c>
       <c r="C469" s="6" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="D469" s="11" t="s">
         <v>71</v>
@@ -8177,10 +8189,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B472" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="D472" s="10" t="s">
         <v>71</v>
@@ -8188,10 +8200,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B473" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C473" s="6" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="D473" s="10" t="s">
         <v>71</v>
@@ -8199,10 +8211,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B474" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C474" s="6" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="D474" s="10" t="s">
         <v>71</v>
@@ -8210,10 +8222,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B475" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C475" s="6" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="D475" s="10" t="s">
         <v>71</v>
@@ -8221,10 +8233,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B476" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C476" s="6" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="D476" s="10" t="s">
         <v>71</v>
@@ -8232,10 +8244,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B477" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C477" s="6" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="D477" s="10" t="s">
         <v>71</v>
@@ -8243,10 +8255,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B478" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C478" s="6" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="D478" s="10" t="s">
         <v>71</v>
@@ -8254,10 +8266,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B479" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C479" s="6" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="D479" s="10" t="s">
         <v>71</v>
@@ -8265,10 +8277,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B480" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C480" s="6" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="D480" s="10" t="s">
         <v>71</v>
@@ -8276,10 +8288,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="5" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C481" s="6" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="D481" s="10" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Done with it for now. Need to review and find new problems.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="887">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -2686,16 +2686,31 @@
     <t xml:space="preserve">Find position of the only set bit</t>
   </si>
   <si>
+    <t xml:space="preserve">use power of 2 concept</t>
+  </si>
+  <si>
     <t xml:space="preserve">Copy set bits in a range</t>
   </si>
   <si>
+    <t xml:space="preserve">use bitmask method</t>
+  </si>
+  <si>
     <t xml:space="preserve">Divide two integers without using multiplication, division and mod operator</t>
   </si>
   <si>
+    <t xml:space="preserve">successive substraction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Calculate square of a number without using *, / and pow()</t>
   </si>
   <si>
+    <t xml:space="preserve">find set bits and perform addition after shifting</t>
+  </si>
+  <si>
     <t xml:space="preserve">Power Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find 2 ^ n strings</t>
   </si>
 </sst>
 </file>
@@ -3230,8 +3245,8 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A454" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D472" activeCellId="0" sqref="D472:D476"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A460" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D479" activeCellId="0" sqref="D479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8267,8 +8282,8 @@
       <c r="C477" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D477" s="11" t="s">
-        <v>71</v>
+      <c r="D477" s="7" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8276,21 +8291,21 @@
         <v>866</v>
       </c>
       <c r="C478" s="6" t="s">
-        <v>878</v>
-      </c>
-      <c r="D478" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="479" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>879</v>
+      </c>
+      <c r="D478" s="7" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B479" s="5" t="s">
         <v>866</v>
       </c>
       <c r="C479" s="6" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D479" s="11" t="s">
-        <v>71</v>
+        <v>882</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8298,21 +8313,21 @@
         <v>866</v>
       </c>
       <c r="C480" s="6" t="s">
-        <v>880</v>
-      </c>
-      <c r="D480" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="481" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>883</v>
+      </c>
+      <c r="D480" s="7" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="5" t="s">
         <v>866</v>
       </c>
       <c r="C481" s="6" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="D481" s="11" t="s">
-        <v>71</v>
+        <v>886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished all Bit Manipulation Sums including new ones.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="921">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -2795,6 +2795,24 @@
   </si>
   <si>
     <t xml:space="preserve">bit wise count number with set bits and unset bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse a number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left shift reverse and right shift number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum XOR Pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">either use sort method or trie method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find nth binary palindrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find len, offset then, calculate using reverse method</t>
   </si>
 </sst>
 </file>
@@ -3327,10 +3345,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D496"/>
+  <dimension ref="A1:D499"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A476" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D496" activeCellId="0" sqref="D496"/>
+      <selection pane="topLeft" activeCell="D499" activeCellId="0" sqref="D499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8572,8 +8590,41 @@
       <c r="B496" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="C496" s="6"/>
-      <c r="D496" s="7"/>
+      <c r="C496" s="6" t="s">
+        <v>915</v>
+      </c>
+      <c r="D496" s="7" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B497" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C497" s="6" t="s">
+        <v>917</v>
+      </c>
+      <c r="D497" s="7" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B498" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C498" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="D498" s="7" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B499" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C499" s="6"/>
+      <c r="D499" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9037,6 +9088,9 @@
     <hyperlink ref="C493" r:id="rId458" display="Find number occuring once where others occur thrice"/>
     <hyperlink ref="C494" r:id="rId459" display="Swap all even and odd bits"/>
     <hyperlink ref="C495" r:id="rId460" display="Sum of bit differences"/>
+    <hyperlink ref="C496" r:id="rId461" display="Reverse a number"/>
+    <hyperlink ref="C497" r:id="rId462" display="Minimum XOR Pair"/>
+    <hyperlink ref="C498" r:id="rId463" display="Find nth binary palindrome"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added Some missing sums
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -3269,7 +3269,7 @@
     <cellStyle name="Card TL" xfId="29"/>
     <cellStyle name="Card TR" xfId="30"/>
     <cellStyle name="Column Header" xfId="31"/>
-    <cellStyle name="Heading1" xfId="32"/>
+    <cellStyle name="Heading 1" xfId="32"/>
     <cellStyle name="Input" xfId="33"/>
     <cellStyle name="Result2" xfId="34"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A476" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D499" activeCellId="0" sqref="D499"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9094,7 +9094,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added Some missing sums from Array and Matrix
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -3269,7 +3269,7 @@
     <cellStyle name="Card TL" xfId="29"/>
     <cellStyle name="Card TR" xfId="30"/>
     <cellStyle name="Column Header" xfId="31"/>
-    <cellStyle name="Heading 1" xfId="32"/>
+    <cellStyle name="Heading 1 1" xfId="32"/>
     <cellStyle name="Input" xfId="33"/>
     <cellStyle name="Result2" xfId="34"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added some missing string sums
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added ChooseAndSwap and new algorithm to compute product array
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -613,7 +613,7 @@
     <t xml:space="preserve">Product array Puzzle</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes/ count zeroes</t>
+    <t xml:space="preserve">Yes/ result = left_product * right_product</t>
   </si>
   <si>
     <t xml:space="preserve">Sort array according to count of set bits</t>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A217" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C227" activeCellId="0" sqref="C227"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D116" activeCellId="0" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4566,7 +4566,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="5" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
Added some practice sums
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -1336,7 +1336,7 @@
     <t xml:space="preserve">Greedy Algorithm to find Minimum number of Coins</t>
   </si>
   <si>
-    <t xml:space="preserve">find minimum, remove coin from pile - min - k</t>
+    <t xml:space="preserve">sort then select the second max leaving small for bob</t>
   </si>
   <si>
     <t xml:space="preserve">Maximum trains for which stoppage can be provided</t>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D116" activeCellId="0" sqref="D116"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A227" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D243" activeCellId="0" sqref="D243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5907,7 +5907,7 @@
       <c r="C243" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="D243" s="11" t="s">
+      <c r="D243" s="7" t="s">
         <v>438</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed tug of war
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -1570,7 +1570,7 @@
     <t xml:space="preserve">Tug of War</t>
   </si>
   <si>
-    <t xml:space="preserve">minDiff = sum/2 - currentSum, if N/2 - nSelected &gt; remaining, return</t>
+    <t xml:space="preserve">backtrack if first.size &lt; n+1 / 2, second.size &lt; n – 1 / 2</t>
   </si>
   <si>
     <t xml:space="preserve">Find shortest safe route in a path with landmines</t>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A227" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D243" activeCellId="0" sqref="D243"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A275" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D284" activeCellId="0" sqref="D284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6337,7 +6337,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="5" t="s">
         <v>496</v>
       </c>

</xml_diff>